<commit_message>
Added data for height. Calculate imc
</commit_message>
<xml_diff>
--- a/data_chart/Ninas.xlsx
+++ b/data_chart/Ninas.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TrabajoDeGrado\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DCD6DC43-7EC0-466D-AA80-7A4B2314F094}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="z-scoresPesoNinas-Semanas" sheetId="1" r:id="rId1"/>
+    <sheet name="z-scoresLongitudNinas-Semanas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Day</t>
   </si>
@@ -59,8 +61,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,8 +81,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,8 +113,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -105,11 +134,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -120,6 +177,27 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +511,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
@@ -7933,4 +8011,1631 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88315F79-66C9-4139-96D6-23FB44563A2A}">
+  <dimension ref="A1:H62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>43.6</v>
+      </c>
+      <c r="C2" s="8">
+        <v>45.4</v>
+      </c>
+      <c r="D2" s="8">
+        <v>47.3</v>
+      </c>
+      <c r="E2" s="9">
+        <v>49.1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>51</v>
+      </c>
+      <c r="G2" s="8">
+        <v>52.9</v>
+      </c>
+      <c r="H2" s="8">
+        <v>54.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>47.8</v>
+      </c>
+      <c r="C3" s="8">
+        <v>49.8</v>
+      </c>
+      <c r="D3" s="8">
+        <v>51.7</v>
+      </c>
+      <c r="E3" s="9">
+        <v>53.7</v>
+      </c>
+      <c r="F3" s="8">
+        <v>55.6</v>
+      </c>
+      <c r="G3" s="8">
+        <v>57.6</v>
+      </c>
+      <c r="H3" s="8">
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
+        <v>51</v>
+      </c>
+      <c r="C4" s="8">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8">
+        <v>55</v>
+      </c>
+      <c r="E4" s="9">
+        <v>57.1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>59.1</v>
+      </c>
+      <c r="G4" s="8">
+        <v>61.1</v>
+      </c>
+      <c r="H4" s="8">
+        <v>63.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <v>53.5</v>
+      </c>
+      <c r="C5" s="8">
+        <v>55.6</v>
+      </c>
+      <c r="D5" s="8">
+        <v>57.7</v>
+      </c>
+      <c r="E5" s="9">
+        <v>59.8</v>
+      </c>
+      <c r="F5" s="8">
+        <v>61.9</v>
+      </c>
+      <c r="G5" s="8">
+        <v>64</v>
+      </c>
+      <c r="H5" s="8">
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8">
+        <v>55.6</v>
+      </c>
+      <c r="C6" s="8">
+        <v>57.8</v>
+      </c>
+      <c r="D6" s="8">
+        <v>59.9</v>
+      </c>
+      <c r="E6" s="9">
+        <v>62.1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>64.3</v>
+      </c>
+      <c r="G6" s="8">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="H6" s="8">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
+        <v>57.4</v>
+      </c>
+      <c r="C7" s="8">
+        <v>59.6</v>
+      </c>
+      <c r="D7" s="8">
+        <v>61.8</v>
+      </c>
+      <c r="E7" s="9">
+        <v>64</v>
+      </c>
+      <c r="F7" s="8">
+        <v>66.2</v>
+      </c>
+      <c r="G7" s="8">
+        <v>68.5</v>
+      </c>
+      <c r="H7" s="8">
+        <v>70.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8">
+        <v>58.9</v>
+      </c>
+      <c r="C8" s="8">
+        <v>61.2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>63.5</v>
+      </c>
+      <c r="E8" s="9">
+        <v>65.7</v>
+      </c>
+      <c r="F8" s="8">
+        <v>68</v>
+      </c>
+      <c r="G8" s="8">
+        <v>70.3</v>
+      </c>
+      <c r="H8" s="8">
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8">
+        <v>60.3</v>
+      </c>
+      <c r="C9" s="8">
+        <v>62.7</v>
+      </c>
+      <c r="D9" s="8">
+        <v>65</v>
+      </c>
+      <c r="E9" s="9">
+        <v>67.3</v>
+      </c>
+      <c r="F9" s="8">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="G9" s="8">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="H9" s="8">
+        <v>74.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8">
+        <v>61.7</v>
+      </c>
+      <c r="C10" s="8">
+        <v>64</v>
+      </c>
+      <c r="D10" s="8">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="E10" s="9">
+        <v>68.7</v>
+      </c>
+      <c r="F10" s="8">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="G10" s="8">
+        <v>73.5</v>
+      </c>
+      <c r="H10" s="8">
+        <v>75.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8">
+        <v>62.9</v>
+      </c>
+      <c r="C11" s="8">
+        <v>65.3</v>
+      </c>
+      <c r="D11" s="8">
+        <v>67.7</v>
+      </c>
+      <c r="E11" s="9">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="F11" s="8">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="G11" s="8">
+        <v>75</v>
+      </c>
+      <c r="H11" s="8">
+        <v>77.400000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="C12" s="8">
+        <v>66.5</v>
+      </c>
+      <c r="D12" s="8">
+        <v>69</v>
+      </c>
+      <c r="E12" s="9">
+        <v>71.5</v>
+      </c>
+      <c r="F12" s="8">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="G12" s="8">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="H12" s="8">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8">
+        <v>65.2</v>
+      </c>
+      <c r="C13" s="8">
+        <v>67.7</v>
+      </c>
+      <c r="D13" s="8">
+        <v>70.3</v>
+      </c>
+      <c r="E13" s="9">
+        <v>72.8</v>
+      </c>
+      <c r="F13" s="8">
+        <v>75.3</v>
+      </c>
+      <c r="G13" s="8">
+        <v>77.8</v>
+      </c>
+      <c r="H13" s="8">
+        <v>80.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8">
+        <v>66.3</v>
+      </c>
+      <c r="C14" s="8">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="D14" s="8">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="E14" s="9">
+        <v>74</v>
+      </c>
+      <c r="F14" s="8">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="G14" s="8">
+        <v>79.2</v>
+      </c>
+      <c r="H14" s="8">
+        <v>81.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8">
+        <v>67.3</v>
+      </c>
+      <c r="C15" s="8">
+        <v>70</v>
+      </c>
+      <c r="D15" s="8">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="E15" s="9">
+        <v>75.2</v>
+      </c>
+      <c r="F15" s="8">
+        <v>77.8</v>
+      </c>
+      <c r="G15" s="8">
+        <v>80.5</v>
+      </c>
+      <c r="H15" s="8">
+        <v>83.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8">
+        <v>68.3</v>
+      </c>
+      <c r="C16" s="8">
+        <v>71</v>
+      </c>
+      <c r="D16" s="8">
+        <v>73.7</v>
+      </c>
+      <c r="E16" s="9">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="F16" s="8">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="G16" s="8">
+        <v>81.7</v>
+      </c>
+      <c r="H16" s="8">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8">
+        <v>69.3</v>
+      </c>
+      <c r="C17" s="8">
+        <v>72</v>
+      </c>
+      <c r="D17" s="8">
+        <v>74.8</v>
+      </c>
+      <c r="E17" s="9">
+        <v>77.5</v>
+      </c>
+      <c r="F17" s="8">
+        <v>80.2</v>
+      </c>
+      <c r="G17" s="8">
+        <v>83</v>
+      </c>
+      <c r="H17" s="8">
+        <v>85.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8">
+        <v>70.2</v>
+      </c>
+      <c r="C18" s="8">
+        <v>73</v>
+      </c>
+      <c r="D18" s="8">
+        <v>75.8</v>
+      </c>
+      <c r="E18" s="9">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="F18" s="8">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="G18" s="8">
+        <v>84.2</v>
+      </c>
+      <c r="H18" s="8">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>17</v>
+      </c>
+      <c r="B19" s="8">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="C19" s="8">
+        <v>74</v>
+      </c>
+      <c r="D19" s="8">
+        <v>76.8</v>
+      </c>
+      <c r="E19" s="9">
+        <v>79.7</v>
+      </c>
+      <c r="F19" s="8">
+        <v>82.5</v>
+      </c>
+      <c r="G19" s="8">
+        <v>85.4</v>
+      </c>
+      <c r="H19" s="8">
+        <v>88.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>18</v>
+      </c>
+      <c r="B20" s="8">
+        <v>72</v>
+      </c>
+      <c r="C20" s="8">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="D20" s="8">
+        <v>77.8</v>
+      </c>
+      <c r="E20" s="9">
+        <v>80.7</v>
+      </c>
+      <c r="F20" s="8">
+        <v>83.6</v>
+      </c>
+      <c r="G20" s="8">
+        <v>86.5</v>
+      </c>
+      <c r="H20" s="8">
+        <v>89.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>19</v>
+      </c>
+      <c r="B21" s="8">
+        <v>72.8</v>
+      </c>
+      <c r="C21" s="8">
+        <v>75.8</v>
+      </c>
+      <c r="D21" s="8">
+        <v>78.8</v>
+      </c>
+      <c r="E21" s="9">
+        <v>81.7</v>
+      </c>
+      <c r="F21" s="8">
+        <v>84.7</v>
+      </c>
+      <c r="G21" s="8">
+        <v>87.6</v>
+      </c>
+      <c r="H21" s="8">
+        <v>90.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>20</v>
+      </c>
+      <c r="B22" s="8">
+        <v>73.7</v>
+      </c>
+      <c r="C22" s="8">
+        <v>76.7</v>
+      </c>
+      <c r="D22" s="8">
+        <v>79.7</v>
+      </c>
+      <c r="E22" s="9">
+        <v>82.7</v>
+      </c>
+      <c r="F22" s="8">
+        <v>85.7</v>
+      </c>
+      <c r="G22" s="8">
+        <v>88.7</v>
+      </c>
+      <c r="H22" s="8">
+        <v>91.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="8">
+        <v>74.5</v>
+      </c>
+      <c r="C23" s="8">
+        <v>77.5</v>
+      </c>
+      <c r="D23" s="8">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="E23" s="9">
+        <v>83.7</v>
+      </c>
+      <c r="F23" s="8">
+        <v>86.7</v>
+      </c>
+      <c r="G23" s="8">
+        <v>89.8</v>
+      </c>
+      <c r="H23" s="8">
+        <v>92.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>22</v>
+      </c>
+      <c r="B24" s="8">
+        <v>75.2</v>
+      </c>
+      <c r="C24" s="8">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="D24" s="8">
+        <v>81.5</v>
+      </c>
+      <c r="E24" s="9">
+        <v>84.6</v>
+      </c>
+      <c r="F24" s="8">
+        <v>87.7</v>
+      </c>
+      <c r="G24" s="8">
+        <v>90.8</v>
+      </c>
+      <c r="H24" s="8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="8">
+        <v>76</v>
+      </c>
+      <c r="C25" s="8">
+        <v>79.2</v>
+      </c>
+      <c r="D25" s="8">
+        <v>82.3</v>
+      </c>
+      <c r="E25" s="9">
+        <v>85.5</v>
+      </c>
+      <c r="F25" s="8">
+        <v>88.7</v>
+      </c>
+      <c r="G25" s="8">
+        <v>91.9</v>
+      </c>
+      <c r="H25" s="8">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>24</v>
+      </c>
+      <c r="B26" s="11">
+        <v>76</v>
+      </c>
+      <c r="C26" s="11">
+        <v>79.3</v>
+      </c>
+      <c r="D26" s="11">
+        <v>82.5</v>
+      </c>
+      <c r="E26" s="11">
+        <v>85.7</v>
+      </c>
+      <c r="F26" s="11">
+        <v>88.9</v>
+      </c>
+      <c r="G26" s="11">
+        <v>92.2</v>
+      </c>
+      <c r="H26" s="11">
+        <v>95.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>25</v>
+      </c>
+      <c r="B27" s="12">
+        <v>76.8</v>
+      </c>
+      <c r="C27" s="8">
+        <v>80</v>
+      </c>
+      <c r="D27" s="8">
+        <v>83.3</v>
+      </c>
+      <c r="E27" s="9">
+        <v>86.6</v>
+      </c>
+      <c r="F27" s="8">
+        <v>89.9</v>
+      </c>
+      <c r="G27" s="8">
+        <v>93.1</v>
+      </c>
+      <c r="H27" s="8">
+        <v>96.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>26</v>
+      </c>
+      <c r="B28" s="12">
+        <v>77.5</v>
+      </c>
+      <c r="C28" s="8">
+        <v>80.8</v>
+      </c>
+      <c r="D28" s="8">
+        <v>84.1</v>
+      </c>
+      <c r="E28" s="9">
+        <v>87.4</v>
+      </c>
+      <c r="F28" s="8">
+        <v>90.8</v>
+      </c>
+      <c r="G28" s="8">
+        <v>94.1</v>
+      </c>
+      <c r="H28" s="8">
+        <v>97.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>27</v>
+      </c>
+      <c r="B29" s="12">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="C29" s="8">
+        <v>81.5</v>
+      </c>
+      <c r="D29" s="8">
+        <v>84.9</v>
+      </c>
+      <c r="E29" s="9">
+        <v>88.3</v>
+      </c>
+      <c r="F29" s="8">
+        <v>91.7</v>
+      </c>
+      <c r="G29" s="8">
+        <v>95</v>
+      </c>
+      <c r="H29" s="8">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>28</v>
+      </c>
+      <c r="B30" s="12">
+        <v>78.8</v>
+      </c>
+      <c r="C30" s="8">
+        <v>82.2</v>
+      </c>
+      <c r="D30" s="8">
+        <v>85.7</v>
+      </c>
+      <c r="E30" s="9">
+        <v>89.1</v>
+      </c>
+      <c r="F30" s="8">
+        <v>92.5</v>
+      </c>
+      <c r="G30" s="8">
+        <v>96</v>
+      </c>
+      <c r="H30" s="8">
+        <v>99.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>29</v>
+      </c>
+      <c r="B31" s="12">
+        <v>79.5</v>
+      </c>
+      <c r="C31" s="8">
+        <v>82.9</v>
+      </c>
+      <c r="D31" s="8">
+        <v>86.4</v>
+      </c>
+      <c r="E31" s="9">
+        <v>89.9</v>
+      </c>
+      <c r="F31" s="8">
+        <v>93.4</v>
+      </c>
+      <c r="G31" s="8">
+        <v>96.9</v>
+      </c>
+      <c r="H31" s="8">
+        <v>100.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>30</v>
+      </c>
+      <c r="B32" s="12">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="C32" s="8">
+        <v>83.6</v>
+      </c>
+      <c r="D32" s="8">
+        <v>87.1</v>
+      </c>
+      <c r="E32" s="9">
+        <v>90.7</v>
+      </c>
+      <c r="F32" s="8">
+        <v>94.2</v>
+      </c>
+      <c r="G32" s="8">
+        <v>97.7</v>
+      </c>
+      <c r="H32" s="8">
+        <v>101.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="12">
+        <v>80.7</v>
+      </c>
+      <c r="C33" s="8">
+        <v>84.3</v>
+      </c>
+      <c r="D33" s="8">
+        <v>87.9</v>
+      </c>
+      <c r="E33" s="9">
+        <v>91.4</v>
+      </c>
+      <c r="F33" s="8">
+        <v>95</v>
+      </c>
+      <c r="G33" s="8">
+        <v>98.6</v>
+      </c>
+      <c r="H33" s="8">
+        <v>102.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>32</v>
+      </c>
+      <c r="B34" s="12">
+        <v>81.3</v>
+      </c>
+      <c r="C34" s="8">
+        <v>84.9</v>
+      </c>
+      <c r="D34" s="8">
+        <v>88.6</v>
+      </c>
+      <c r="E34" s="9">
+        <v>92.2</v>
+      </c>
+      <c r="F34" s="8">
+        <v>95.8</v>
+      </c>
+      <c r="G34" s="8">
+        <v>99.4</v>
+      </c>
+      <c r="H34" s="8">
+        <v>103.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>33</v>
+      </c>
+      <c r="B35" s="12">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="C35" s="8">
+        <v>85.6</v>
+      </c>
+      <c r="D35" s="8">
+        <v>89.3</v>
+      </c>
+      <c r="E35" s="9">
+        <v>92.9</v>
+      </c>
+      <c r="F35" s="8">
+        <v>96.6</v>
+      </c>
+      <c r="G35" s="8">
+        <v>100.3</v>
+      </c>
+      <c r="H35" s="8">
+        <v>103.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>34</v>
+      </c>
+      <c r="B36" s="12">
+        <v>82.5</v>
+      </c>
+      <c r="C36" s="8">
+        <v>86.2</v>
+      </c>
+      <c r="D36" s="8">
+        <v>89.9</v>
+      </c>
+      <c r="E36" s="9">
+        <v>93.6</v>
+      </c>
+      <c r="F36" s="8">
+        <v>97.4</v>
+      </c>
+      <c r="G36" s="8">
+        <v>101.1</v>
+      </c>
+      <c r="H36" s="8">
+        <v>104.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>35</v>
+      </c>
+      <c r="B37" s="12">
+        <v>83.1</v>
+      </c>
+      <c r="C37" s="8">
+        <v>86.8</v>
+      </c>
+      <c r="D37" s="8">
+        <v>90.6</v>
+      </c>
+      <c r="E37" s="9">
+        <v>94.4</v>
+      </c>
+      <c r="F37" s="8">
+        <v>98.1</v>
+      </c>
+      <c r="G37" s="8">
+        <v>101.9</v>
+      </c>
+      <c r="H37" s="8">
+        <v>105.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>36</v>
+      </c>
+      <c r="B38" s="12">
+        <v>83.6</v>
+      </c>
+      <c r="C38" s="8">
+        <v>87.4</v>
+      </c>
+      <c r="D38" s="8">
+        <v>91.2</v>
+      </c>
+      <c r="E38" s="9">
+        <v>95.1</v>
+      </c>
+      <c r="F38" s="8">
+        <v>98.9</v>
+      </c>
+      <c r="G38" s="8">
+        <v>102.7</v>
+      </c>
+      <c r="H38" s="8">
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>37</v>
+      </c>
+      <c r="B39" s="12">
+        <v>84.2</v>
+      </c>
+      <c r="C39" s="8">
+        <v>88</v>
+      </c>
+      <c r="D39" s="8">
+        <v>91.9</v>
+      </c>
+      <c r="E39" s="9">
+        <v>95.7</v>
+      </c>
+      <c r="F39" s="8">
+        <v>99.6</v>
+      </c>
+      <c r="G39" s="8">
+        <v>103.4</v>
+      </c>
+      <c r="H39" s="8">
+        <v>107.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>38</v>
+      </c>
+      <c r="B40" s="12">
+        <v>84.7</v>
+      </c>
+      <c r="C40" s="8">
+        <v>88.6</v>
+      </c>
+      <c r="D40" s="8">
+        <v>92.5</v>
+      </c>
+      <c r="E40" s="9">
+        <v>96.4</v>
+      </c>
+      <c r="F40" s="8">
+        <v>100.3</v>
+      </c>
+      <c r="G40" s="8">
+        <v>104.2</v>
+      </c>
+      <c r="H40" s="8">
+        <v>108.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>39</v>
+      </c>
+      <c r="B41" s="12">
+        <v>85.3</v>
+      </c>
+      <c r="C41" s="8">
+        <v>89.2</v>
+      </c>
+      <c r="D41" s="8">
+        <v>93.1</v>
+      </c>
+      <c r="E41" s="9">
+        <v>97.1</v>
+      </c>
+      <c r="F41" s="8">
+        <v>101</v>
+      </c>
+      <c r="G41" s="8">
+        <v>105</v>
+      </c>
+      <c r="H41" s="8">
+        <v>108.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>40</v>
+      </c>
+      <c r="B42" s="12">
+        <v>85.8</v>
+      </c>
+      <c r="C42" s="8">
+        <v>89.8</v>
+      </c>
+      <c r="D42" s="8">
+        <v>93.8</v>
+      </c>
+      <c r="E42" s="9">
+        <v>97.7</v>
+      </c>
+      <c r="F42" s="8">
+        <v>101.7</v>
+      </c>
+      <c r="G42" s="8">
+        <v>105.7</v>
+      </c>
+      <c r="H42" s="8">
+        <v>109.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>41</v>
+      </c>
+      <c r="B43" s="12">
+        <v>86.3</v>
+      </c>
+      <c r="C43" s="8">
+        <v>90.4</v>
+      </c>
+      <c r="D43" s="8">
+        <v>94.4</v>
+      </c>
+      <c r="E43" s="9">
+        <v>98.4</v>
+      </c>
+      <c r="F43" s="8">
+        <v>102.4</v>
+      </c>
+      <c r="G43" s="8">
+        <v>106.4</v>
+      </c>
+      <c r="H43" s="8">
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>42</v>
+      </c>
+      <c r="B44" s="12">
+        <v>86.8</v>
+      </c>
+      <c r="C44" s="8">
+        <v>90.9</v>
+      </c>
+      <c r="D44" s="8">
+        <v>95</v>
+      </c>
+      <c r="E44" s="9">
+        <v>99</v>
+      </c>
+      <c r="F44" s="8">
+        <v>103.1</v>
+      </c>
+      <c r="G44" s="8">
+        <v>107.2</v>
+      </c>
+      <c r="H44" s="8">
+        <v>111.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>43</v>
+      </c>
+      <c r="B45" s="12">
+        <v>87.4</v>
+      </c>
+      <c r="C45" s="8">
+        <v>91.5</v>
+      </c>
+      <c r="D45" s="8">
+        <v>95.6</v>
+      </c>
+      <c r="E45" s="9">
+        <v>99.7</v>
+      </c>
+      <c r="F45" s="8">
+        <v>103.8</v>
+      </c>
+      <c r="G45" s="8">
+        <v>107.9</v>
+      </c>
+      <c r="H45" s="8">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>44</v>
+      </c>
+      <c r="B46" s="12">
+        <v>87.9</v>
+      </c>
+      <c r="C46" s="8">
+        <v>92</v>
+      </c>
+      <c r="D46" s="8">
+        <v>96.2</v>
+      </c>
+      <c r="E46" s="9">
+        <v>100.3</v>
+      </c>
+      <c r="F46" s="8">
+        <v>104.5</v>
+      </c>
+      <c r="G46" s="8">
+        <v>108.6</v>
+      </c>
+      <c r="H46" s="8">
+        <v>112.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>45</v>
+      </c>
+      <c r="B47" s="12">
+        <v>88.4</v>
+      </c>
+      <c r="C47" s="8">
+        <v>92.5</v>
+      </c>
+      <c r="D47" s="8">
+        <v>96.7</v>
+      </c>
+      <c r="E47" s="9">
+        <v>100.9</v>
+      </c>
+      <c r="F47" s="8">
+        <v>105.1</v>
+      </c>
+      <c r="G47" s="8">
+        <v>109.3</v>
+      </c>
+      <c r="H47" s="8">
+        <v>113.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>46</v>
+      </c>
+      <c r="B48" s="12">
+        <v>88.9</v>
+      </c>
+      <c r="C48" s="8">
+        <v>93.1</v>
+      </c>
+      <c r="D48" s="8">
+        <v>97.3</v>
+      </c>
+      <c r="E48" s="9">
+        <v>101.5</v>
+      </c>
+      <c r="F48" s="8">
+        <v>105.8</v>
+      </c>
+      <c r="G48" s="8">
+        <v>110</v>
+      </c>
+      <c r="H48" s="8">
+        <v>114.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>47</v>
+      </c>
+      <c r="B49" s="12">
+        <v>89.3</v>
+      </c>
+      <c r="C49" s="8">
+        <v>93.6</v>
+      </c>
+      <c r="D49" s="8">
+        <v>97.9</v>
+      </c>
+      <c r="E49" s="9">
+        <v>102.1</v>
+      </c>
+      <c r="F49" s="8">
+        <v>106.4</v>
+      </c>
+      <c r="G49" s="8">
+        <v>110.7</v>
+      </c>
+      <c r="H49" s="8">
+        <v>114.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>48</v>
+      </c>
+      <c r="B50" s="12">
+        <v>89.8</v>
+      </c>
+      <c r="C50" s="8">
+        <v>94.1</v>
+      </c>
+      <c r="D50" s="8">
+        <v>98.4</v>
+      </c>
+      <c r="E50" s="9">
+        <v>102.7</v>
+      </c>
+      <c r="F50" s="8">
+        <v>107</v>
+      </c>
+      <c r="G50" s="8">
+        <v>111.3</v>
+      </c>
+      <c r="H50" s="8">
+        <v>115.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>49</v>
+      </c>
+      <c r="B51" s="12">
+        <v>90.3</v>
+      </c>
+      <c r="C51" s="8">
+        <v>94.6</v>
+      </c>
+      <c r="D51" s="8">
+        <v>99</v>
+      </c>
+      <c r="E51" s="9">
+        <v>103.3</v>
+      </c>
+      <c r="F51" s="8">
+        <v>107.7</v>
+      </c>
+      <c r="G51" s="8">
+        <v>112</v>
+      </c>
+      <c r="H51" s="8">
+        <v>116.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>50</v>
+      </c>
+      <c r="B52" s="12">
+        <v>90.7</v>
+      </c>
+      <c r="C52" s="8">
+        <v>95.1</v>
+      </c>
+      <c r="D52" s="8">
+        <v>99.5</v>
+      </c>
+      <c r="E52" s="9">
+        <v>103.9</v>
+      </c>
+      <c r="F52" s="8">
+        <v>108.3</v>
+      </c>
+      <c r="G52" s="8">
+        <v>112.7</v>
+      </c>
+      <c r="H52" s="8">
+        <v>117.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>51</v>
+      </c>
+      <c r="B53" s="12">
+        <v>91.2</v>
+      </c>
+      <c r="C53" s="8">
+        <v>95.6</v>
+      </c>
+      <c r="D53" s="8">
+        <v>100.1</v>
+      </c>
+      <c r="E53" s="9">
+        <v>104.5</v>
+      </c>
+      <c r="F53" s="8">
+        <v>108.9</v>
+      </c>
+      <c r="G53" s="8">
+        <v>113.3</v>
+      </c>
+      <c r="H53" s="8">
+        <v>117.7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>52</v>
+      </c>
+      <c r="B54" s="12">
+        <v>91.7</v>
+      </c>
+      <c r="C54" s="8">
+        <v>96.1</v>
+      </c>
+      <c r="D54" s="8">
+        <v>100.6</v>
+      </c>
+      <c r="E54" s="9">
+        <v>105</v>
+      </c>
+      <c r="F54" s="8">
+        <v>109.5</v>
+      </c>
+      <c r="G54" s="8">
+        <v>114</v>
+      </c>
+      <c r="H54" s="8">
+        <v>118.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>53</v>
+      </c>
+      <c r="B55" s="12">
+        <v>92.1</v>
+      </c>
+      <c r="C55" s="8">
+        <v>96.6</v>
+      </c>
+      <c r="D55" s="8">
+        <v>101.1</v>
+      </c>
+      <c r="E55" s="9">
+        <v>105.6</v>
+      </c>
+      <c r="F55" s="8">
+        <v>110.1</v>
+      </c>
+      <c r="G55" s="8">
+        <v>114.6</v>
+      </c>
+      <c r="H55" s="8">
+        <v>119.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>54</v>
+      </c>
+      <c r="B56" s="12">
+        <v>92.6</v>
+      </c>
+      <c r="C56" s="8">
+        <v>97.1</v>
+      </c>
+      <c r="D56" s="8">
+        <v>101.6</v>
+      </c>
+      <c r="E56" s="9">
+        <v>106.2</v>
+      </c>
+      <c r="F56" s="8">
+        <v>110.7</v>
+      </c>
+      <c r="G56" s="8">
+        <v>115.2</v>
+      </c>
+      <c r="H56" s="8">
+        <v>119.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
+        <v>55</v>
+      </c>
+      <c r="B57" s="12">
+        <v>93</v>
+      </c>
+      <c r="C57" s="8">
+        <v>97.6</v>
+      </c>
+      <c r="D57" s="8">
+        <v>102.2</v>
+      </c>
+      <c r="E57" s="9">
+        <v>106.7</v>
+      </c>
+      <c r="F57" s="8">
+        <v>111.3</v>
+      </c>
+      <c r="G57" s="8">
+        <v>115.9</v>
+      </c>
+      <c r="H57" s="8">
+        <v>120.4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>56</v>
+      </c>
+      <c r="B58" s="12">
+        <v>93.4</v>
+      </c>
+      <c r="C58" s="8">
+        <v>98.1</v>
+      </c>
+      <c r="D58" s="8">
+        <v>102.7</v>
+      </c>
+      <c r="E58" s="9">
+        <v>107.3</v>
+      </c>
+      <c r="F58" s="8">
+        <v>111.9</v>
+      </c>
+      <c r="G58" s="8">
+        <v>116.5</v>
+      </c>
+      <c r="H58" s="8">
+        <v>121.1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <v>57</v>
+      </c>
+      <c r="B59" s="12">
+        <v>93.9</v>
+      </c>
+      <c r="C59" s="8">
+        <v>98.5</v>
+      </c>
+      <c r="D59" s="8">
+        <v>103.2</v>
+      </c>
+      <c r="E59" s="9">
+        <v>107.8</v>
+      </c>
+      <c r="F59" s="8">
+        <v>112.5</v>
+      </c>
+      <c r="G59" s="8">
+        <v>117.1</v>
+      </c>
+      <c r="H59" s="8">
+        <v>121.8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <v>58</v>
+      </c>
+      <c r="B60" s="12">
+        <v>94.3</v>
+      </c>
+      <c r="C60" s="8">
+        <v>99</v>
+      </c>
+      <c r="D60" s="8">
+        <v>103.7</v>
+      </c>
+      <c r="E60" s="9">
+        <v>108.4</v>
+      </c>
+      <c r="F60" s="8">
+        <v>113</v>
+      </c>
+      <c r="G60" s="8">
+        <v>117.7</v>
+      </c>
+      <c r="H60" s="8">
+        <v>122.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>59</v>
+      </c>
+      <c r="B61" s="12">
+        <v>94.7</v>
+      </c>
+      <c r="C61" s="8">
+        <v>99.5</v>
+      </c>
+      <c r="D61" s="8">
+        <v>104.2</v>
+      </c>
+      <c r="E61" s="9">
+        <v>108.9</v>
+      </c>
+      <c r="F61" s="8">
+        <v>113.6</v>
+      </c>
+      <c r="G61" s="8">
+        <v>118.3</v>
+      </c>
+      <c r="H61" s="8">
+        <v>123.1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>60</v>
+      </c>
+      <c r="B62" s="12">
+        <v>95.2</v>
+      </c>
+      <c r="C62" s="8">
+        <v>99.9</v>
+      </c>
+      <c r="D62" s="8">
+        <v>104.7</v>
+      </c>
+      <c r="E62" s="9">
+        <v>109.4</v>
+      </c>
+      <c r="F62" s="8">
+        <v>114.2</v>
+      </c>
+      <c r="G62" s="8">
+        <v>118.9</v>
+      </c>
+      <c r="H62" s="8">
+        <v>123.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>